<commit_message>
Added more AA path genes
</commit_message>
<xml_diff>
--- a/Matt_Work/AA paths/All_Paths_formatted.xlsx
+++ b/Matt_Work/AA paths/All_Paths_formatted.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="10500" windowHeight="5832" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="10500" windowHeight="5832" firstSheet="10" activeTab="12"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Summary and notes" sheetId="1" r:id="rId1"/>
     <sheet name="Alanine" sheetId="2" r:id="rId2"/>
     <sheet name="Arginine" sheetId="3" r:id="rId3"/>
     <sheet name="Asparagine" sheetId="4" r:id="rId4"/>
@@ -30,7 +30,7 @@
     <sheet name="Valine" sheetId="21" r:id="rId21"/>
   </sheets>
   <definedNames>
-    <definedName name="All_Paths" localSheetId="0">Sheet1!$A$1:$E$65</definedName>
+    <definedName name="All_Paths" localSheetId="0">'Summary and notes'!$A$1:$E$65</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="401">
   <si>
     <t>Amino Acid Syntheses (** is GOGAT cycle--&gt;rxn00187_c0,rxn00260_c0,rxn00085_c0)</t>
   </si>
@@ -109,9 +109,6 @@
     <t>Cysteine Exactly Serine plus sulfur</t>
   </si>
   <si>
-    <t>**See below for L-Serine</t>
-  </si>
-  <si>
     <t>rxn05909_c0</t>
   </si>
   <si>
@@ -235,9 +232,6 @@
     <t>H2S + O-Succinyl-L-homoserine -&gt; H+ + Homocysteine + Succinate</t>
   </si>
   <si>
-    <t>**See L-Methionine path below</t>
-  </si>
-  <si>
     <t>rxn00126_c0</t>
   </si>
   <si>
@@ -253,9 +247,6 @@
     <t>H2O + S-Adenosyl-homocysteine &lt;=&gt; Homocysteine + Adenosine</t>
   </si>
   <si>
-    <t>rxn04594_c0</t>
-  </si>
-  <si>
     <t xml:space="preserve">H+ + NADH + 5-10-Methylenetetrahydrofolate -&gt; NAD + 5-Methyltetrahydrofolate </t>
   </si>
   <si>
@@ -265,9 +256,6 @@
     <t>Homocysteine + 5-Methyltetrahydrofolate -&gt; L-Methionine + Tetrahydrofolate</t>
   </si>
   <si>
-    <t>**Threonine pathway is below</t>
-  </si>
-  <si>
     <t>rxn01068_c0</t>
   </si>
   <si>
@@ -280,9 +268,6 @@
     <t>CoA + L-2-Amino-acetoacetate -&gt; Acetyl-CoA + Glycine</t>
   </si>
   <si>
-    <t>**Serine pathway is below</t>
-  </si>
-  <si>
     <t>(LESS)rxn00692_c0</t>
   </si>
   <si>
@@ -1015,9 +1000,6 @@
     <t>CoA + Succinate + ATP &lt;=&gt; Phosphate + ADP + Succinyl-CoA</t>
   </si>
   <si>
-    <t>*Need Genes</t>
-  </si>
-  <si>
     <t xml:space="preserve">rxn01637_c0 </t>
   </si>
   <si>
@@ -1121,14 +1103,175 @@
   </si>
   <si>
     <t>(mmp1589 and mmp1013)</t>
+  </si>
+  <si>
+    <t>mmp0918</t>
+  </si>
+  <si>
+    <t>**See Serine</t>
+  </si>
+  <si>
+    <t>mmp0941</t>
+  </si>
+  <si>
+    <t>mmp1681</t>
+  </si>
+  <si>
+    <t>mmp0078</t>
+  </si>
+  <si>
+    <t>mmp0645</t>
+  </si>
+  <si>
+    <t>mmp0130 or mmp1548</t>
+  </si>
+  <si>
+    <t>Fdh</t>
+  </si>
+  <si>
+    <t>(mmp0138 and mmp0139) or (mmp1297 and mmp1298)</t>
+  </si>
+  <si>
+    <t>mmp0123</t>
+  </si>
+  <si>
+    <t>(mmp0178 and (mmp0179 or mmp0882) and mmp0179)</t>
+  </si>
+  <si>
+    <t>mmp1254 or mmp0882</t>
+  </si>
+  <si>
+    <t>mmp0282</t>
+  </si>
+  <si>
+    <t>mmp0540</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmp1277 and mmp1067 </t>
+  </si>
+  <si>
+    <t>mmp0971</t>
+  </si>
+  <si>
+    <t>(mmp1105 and mmp0955)</t>
+  </si>
+  <si>
+    <t>mmp0012</t>
+  </si>
+  <si>
+    <t>mmp1640</t>
+  </si>
+  <si>
+    <t>mmp0920</t>
+  </si>
+  <si>
+    <t>mmp0981</t>
+  </si>
+  <si>
+    <t>**See Methionine path</t>
+  </si>
+  <si>
+    <t>(mmp1151 and mmp0829)</t>
+  </si>
+  <si>
+    <t>**See Threonine path</t>
+  </si>
+  <si>
+    <t>mmp1574</t>
+  </si>
+  <si>
+    <t>**See Serine path</t>
+  </si>
+  <si>
+    <t>mmp0396</t>
+  </si>
+  <si>
+    <t>(mmp0598 or mmp1439 or mmp0112)</t>
+  </si>
+  <si>
+    <t>mmp0945</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(mmp1113 or mmp1115) </t>
+  </si>
+  <si>
+    <t>mmp0968</t>
+  </si>
+  <si>
+    <t>mmp0548</t>
+  </si>
+  <si>
+    <t>(mmp1216 and mmp1527)</t>
+  </si>
+  <si>
+    <t>((mmp0256 or mmp1082) and (mmp1722 or mmp1083))</t>
+  </si>
+  <si>
+    <t>mmp0417</t>
+  </si>
+  <si>
+    <t>(mmp0280 and mmp0051)</t>
+  </si>
+  <si>
+    <t>mmp0947</t>
+  </si>
+  <si>
+    <t>mmp1189</t>
+  </si>
+  <si>
+    <t>mmp1114</t>
+  </si>
+  <si>
+    <t>mmp1018</t>
+  </si>
+  <si>
+    <t>mmp1149</t>
+  </si>
+  <si>
+    <t>mmp1480</t>
+  </si>
+  <si>
+    <t>mmp0539</t>
+  </si>
+  <si>
+    <t>mmp0650 or mmp0651</t>
+  </si>
+  <si>
+    <t>mmp1063</t>
+  </si>
+  <si>
+    <t>(mmp0136 or mmp1149)</t>
+  </si>
+  <si>
+    <t>(mmp1149 and mmp0136)</t>
+  </si>
+  <si>
+    <t>mmp0576</t>
+  </si>
+  <si>
+    <t>mmp0923</t>
+  </si>
+  <si>
+    <t>mmp1527</t>
+  </si>
+  <si>
+    <t>mmp0917</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1156,8 +1299,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1465,8 +1612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66:XFD72"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1496,22 +1643,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="115.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" t="s">
-        <v>310</v>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="1" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1522,7 +1671,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1530,10 +1679,10 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C3" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1544,175 +1693,240 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>317</v>
+        <v>312</v>
+      </c>
+      <c r="C5" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B6" t="s">
-        <v>316</v>
+        <v>311</v>
+      </c>
+      <c r="C6" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B7" t="s">
-        <v>256</v>
+        <v>251</v>
+      </c>
+      <c r="C7" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B8" t="s">
-        <v>315</v>
+        <v>310</v>
+      </c>
+      <c r="C8" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B9" t="s">
-        <v>314</v>
+        <v>309</v>
+      </c>
+      <c r="C9" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B10" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>86</v>
-      </c>
+        <v>308</v>
+      </c>
+      <c r="C10" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B12" t="s">
-        <v>88</v>
+        <v>83</v>
+      </c>
+      <c r="C12" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B13" t="s">
-        <v>90</v>
+        <v>85</v>
+      </c>
+      <c r="C13" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B14" t="s">
-        <v>92</v>
+        <v>87</v>
+      </c>
+      <c r="C14" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B15" t="s">
-        <v>94</v>
+        <v>89</v>
+      </c>
+      <c r="C15" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" t="s">
+        <v>307</v>
+      </c>
+      <c r="C16" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" t="s">
+        <v>306</v>
+      </c>
+      <c r="C17" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" t="s">
         <v>95</v>
       </c>
-      <c r="B16" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="C19" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>96</v>
       </c>
-      <c r="B17" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B20" t="s">
         <v>97</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C20" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="B21" t="s">
         <v>99</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C21" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="B22" t="s">
         <v>101</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C22" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="B23" t="s">
         <v>103</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C23" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="B24" t="s">
         <v>105</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C24" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="B25" t="s">
         <v>107</v>
       </c>
-      <c r="B23" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>109</v>
-      </c>
-      <c r="B24" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>111</v>
-      </c>
-      <c r="B25" t="s">
-        <v>112</v>
+      <c r="C25" t="s">
+        <v>380</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1722,7 +1936,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1733,11 +1947,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>113</v>
+      <c r="A1" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="C1" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1748,7 +1962,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1756,10 +1970,10 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C3" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1770,84 +1984,114 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>114</v>
-      </c>
+      <c r="A5" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B6" t="s">
-        <v>116</v>
+        <v>111</v>
+      </c>
+      <c r="C6" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B7" t="s">
-        <v>118</v>
+        <v>113</v>
+      </c>
+      <c r="C7" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B8" t="s">
-        <v>120</v>
+        <v>115</v>
+      </c>
+      <c r="C8" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B9" t="s">
-        <v>122</v>
+        <v>117</v>
+      </c>
+      <c r="C9" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>123</v>
-      </c>
+      <c r="A10" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B11" t="s">
-        <v>125</v>
+        <v>120</v>
+      </c>
+      <c r="C11" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B12" t="s">
-        <v>127</v>
+        <v>122</v>
+      </c>
+      <c r="C12" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B13" t="s">
-        <v>129</v>
+        <v>124</v>
+      </c>
+      <c r="C13" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B14" t="s">
-        <v>131</v>
+        <v>126</v>
+      </c>
+      <c r="C14" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A5:B5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1857,7 +2101,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1868,11 +2112,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>132</v>
+      <c r="A1" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="C1" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1883,7 +2127,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1891,10 +2135,10 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C3" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1905,95 +2149,126 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>133</v>
-      </c>
+      <c r="A5" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B6" t="s">
-        <v>135</v>
+        <v>130</v>
+      </c>
+      <c r="C6" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B7" t="s">
-        <v>137</v>
+        <v>132</v>
+      </c>
+      <c r="C7" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B8" t="s">
-        <v>139</v>
+        <v>134</v>
+      </c>
+      <c r="C8" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B9" t="s">
-        <v>141</v>
+        <v>136</v>
+      </c>
+      <c r="C9" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B10" t="s">
-        <v>143</v>
+        <v>138</v>
+      </c>
+      <c r="C10" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B11" t="s">
-        <v>145</v>
+        <v>140</v>
+      </c>
+      <c r="C11" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B12" t="s">
-        <v>147</v>
+        <v>142</v>
+      </c>
+      <c r="C12" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B13" t="s">
-        <v>149</v>
+        <v>144</v>
+      </c>
+      <c r="C13" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B14" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B15" t="s">
-        <v>153</v>
+        <v>148</v>
+      </c>
+      <c r="C15" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A5:B5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2002,8 +2277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2014,11 +2289,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>154</v>
+      <c r="A1" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="C1" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -2029,7 +2304,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -2037,10 +2312,10 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C3" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -2051,76 +2326,100 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>155</v>
-      </c>
+      <c r="A5" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
         <v>50</v>
       </c>
-      <c r="B6" t="s">
-        <v>51</v>
+      <c r="C6" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
         <v>52</v>
       </c>
-      <c r="B7" t="s">
-        <v>53</v>
+      <c r="C7" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>156</v>
-      </c>
+      <c r="A8" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B9" t="s">
-        <v>158</v>
+        <v>153</v>
+      </c>
+      <c r="C9" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B10" t="s">
-        <v>160</v>
+        <v>155</v>
+      </c>
+      <c r="C10" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B11" t="s">
-        <v>162</v>
+        <v>157</v>
+      </c>
+      <c r="C11" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B12" t="s">
-        <v>164</v>
+        <v>159</v>
+      </c>
+      <c r="C12" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B13" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A8:B8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2129,8 +2428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2142,10 +2441,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C1" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -2156,7 +2455,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -2164,10 +2463,10 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C3" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -2178,129 +2477,132 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
         <v>50</v>
-      </c>
-      <c r="B5" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
         <v>52</v>
-      </c>
-      <c r="B6" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
         <v>54</v>
-      </c>
-      <c r="B7" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
         <v>34</v>
       </c>
-      <c r="B13" t="s">
-        <v>35</v>
+      <c r="C13" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B15" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B16" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B18" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B19" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B20" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -2325,141 +2627,141 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="C3" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B4" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B5" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="C5" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B6" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C6" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B7" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C7" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B8" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C8" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B9" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C9" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B10" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C10" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B11" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C11" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B12" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B13" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="C13" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B14" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="C14" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -2484,12 +2786,12 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -2497,10 +2799,10 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="C3" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -2508,40 +2810,40 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C4" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B5" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="C5" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B6" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C6" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B7" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -2566,72 +2868,72 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="C4" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="C5" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B6" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="C6" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B7" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="C7" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B8" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="C8" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -2656,67 +2958,67 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="C4" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="C5" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="C6" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B7" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="C7" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="B8" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="C8" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -2741,182 +3043,182 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B3" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="C3" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C5" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B6" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C6" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B7" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="C7" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B8" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C8" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B9" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="C9" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B10" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C10" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B11" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C11" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B12" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C12" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B13" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C13" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B14" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C14" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B15" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="C15" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B16" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="C16" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B17" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="C17" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B18" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="C18" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -2943,7 +3245,7 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -2953,32 +3255,32 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="B3" t="s">
+        <v>333</v>
+      </c>
+      <c r="C3" t="s">
         <v>339</v>
-      </c>
-      <c r="C3" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="B4" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="B5" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="C5" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -3003,152 +3305,152 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="C3" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C4" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B5" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="C5" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B6" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C6" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B7" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="C7" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B8" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C8" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B9" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C9" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B10" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C10" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B11" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C11" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B12" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="C12" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B13" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B14" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C14" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B15" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C15" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -3173,67 +3475,67 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B3" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C3" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B4" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="C4" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B5" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C5" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B6" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="C6" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B7" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C7" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -3245,8 +3547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3261,7 +3563,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -3272,7 +3574,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -3280,13 +3582,13 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="C3" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D3" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -3297,106 +3599,106 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="B5" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="C5" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="B6" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C6" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="B7" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="C7" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="B8" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="C8" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="B9" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="C9" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="B10" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="C10" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="B11" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="C11" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="B12" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="C12" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="B13" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="C13" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -3409,7 +3711,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3424,7 +3726,7 @@
         <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>310</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3435,7 +3737,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -3443,10 +3745,10 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C3" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3457,7 +3759,7 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -3466,6 +3768,9 @@
       </c>
       <c r="B5" t="s">
         <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -3479,7 +3784,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3493,7 +3798,7 @@
         <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>310</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3504,7 +3809,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -3512,10 +3817,10 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C3" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3526,7 +3831,7 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>
@@ -3536,30 +3841,37 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+    <col min="2" max="2" width="29.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -3572,21 +3884,22 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.109375" customWidth="1"/>
     <col min="2" max="2" width="59.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>310</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3597,7 +3910,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -3605,10 +3918,10 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C3" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3619,7 +3932,7 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>
@@ -3632,21 +3945,22 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.5546875" customWidth="1"/>
     <col min="2" max="2" width="59.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>310</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3657,7 +3971,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -3665,10 +3979,10 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C3" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3679,7 +3993,7 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>
@@ -3691,22 +4005,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="102.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" t="s">
-        <v>320</v>
+      <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="1" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3717,7 +4033,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -3725,10 +4041,10 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C3" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3739,243 +4055,321 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" t="s">
-        <v>25</v>
+      <c r="C5" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
         <v>26</v>
       </c>
-      <c r="B6" t="s">
-        <v>27</v>
+      <c r="C6" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" t="s">
-        <v>29</v>
+      <c r="C7" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" t="s">
-        <v>31</v>
+      <c r="C8" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" t="s">
-        <v>33</v>
+      <c r="C9" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>357</v>
+      </c>
+      <c r="B10" t="s">
         <v>34</v>
       </c>
-      <c r="B10" t="s">
-        <v>35</v>
+      <c r="C10" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
         <v>36</v>
       </c>
-      <c r="B11" t="s">
-        <v>37</v>
+      <c r="C11" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
         <v>38</v>
       </c>
-      <c r="B12" t="s">
-        <v>39</v>
+      <c r="C12" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
         <v>40</v>
       </c>
-      <c r="B13" t="s">
-        <v>41</v>
+      <c r="C13" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
         <v>42</v>
       </c>
-      <c r="B14" t="s">
-        <v>43</v>
+      <c r="C14" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
         <v>44</v>
       </c>
-      <c r="B15" t="s">
-        <v>45</v>
+      <c r="C15" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
         <v>46</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
         <v>48</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>313</v>
+      </c>
+      <c r="B18" t="s">
+        <v>314</v>
+      </c>
+      <c r="C18" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>318</v>
-      </c>
-      <c r="B18" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
         <v>50</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
         <v>52</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
         <v>54</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
         <v>56</v>
       </c>
-      <c r="B22" t="s">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="B23" t="s">
         <v>58</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="B25" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="C25" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="B27" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="C27" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>167</v>
+      </c>
+      <c r="B28" t="s">
         <v>64</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C28" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="B29" t="s">
         <v>66</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C29" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="B31" t="s">
         <v>68</v>
       </c>
-      <c r="B29" t="s">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="B32" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>71</v>
-      </c>
-      <c r="B31" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>73</v>
-      </c>
-      <c r="B32" t="s">
-        <v>74</v>
+      <c r="C32" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>75</v>
+      <c r="A33" s="1" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B34" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>78</v>
-      </c>
+      <c r="A35" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A35:B35"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added experimental images and thermo codes
</commit_message>
<xml_diff>
--- a/Matt_Work/AA paths/All_Paths_formatted.xlsx
+++ b/Matt_Work/AA paths/All_Paths_formatted.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="10500" windowHeight="5832" firstSheet="14" activeTab="20"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="10500" windowHeight="5832" firstSheet="9" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Summary and notes" sheetId="1" r:id="rId1"/>
@@ -1308,7 +1308,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1318,6 +1318,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1334,7 +1346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1344,13 +1356,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1702,25 +1716,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>392</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -1975,10 +1989,10 @@
       </c>
     </row>
     <row r="11" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="6"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -2146,8 +2160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2202,10 +2216,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="6"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -2252,10 +2266,10 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="B10" s="5"/>
+      <c r="B10" s="6"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -2315,7 +2329,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2370,10 +2384,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="6"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -2495,7 +2509,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2550,10 +2564,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="6"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -2578,10 +2592,10 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="6"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -2627,14 +2641,14 @@
         <v>386</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="13" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="8" t="s">
         <v>387</v>
       </c>
     </row>
@@ -2651,8 +2665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2751,10 +2765,10 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="6"/>
     </row>
     <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -2808,58 +2822,58 @@
         <v>345</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+    <row r="15" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="5" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+    <row r="16" spans="1:3" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="5" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="6" t="s">
         <v>413</v>
       </c>
-      <c r="B17" s="5"/>
-    </row>
-    <row r="18" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
+      <c r="B17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="5" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+    <row r="19" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="5" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
+    <row r="20" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="5" t="s">
         <v>390</v>
       </c>
     </row>
@@ -2878,7 +2892,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2933,10 +2947,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>414</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="6"/>
     </row>
     <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -3080,7 +3094,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3135,10 +3149,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="6"/>
     </row>
     <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -3173,14 +3187,14 @@
         <v>186</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="8" t="s">
         <v>188</v>
       </c>
     </row>
@@ -3205,13 +3219,13 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="123.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="123.6640625" customWidth="1"/>
     <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3260,16 +3274,16 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="6"/>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>411</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="6"/>
     </row>
     <row r="7" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
@@ -3395,14 +3409,14 @@
         <v>197</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="16" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="9" t="s">
         <v>199</v>
       </c>
     </row>
@@ -3420,7 +3434,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3475,10 +3489,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="6"/>
     </row>
     <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -3524,14 +3538,14 @@
         <v>206</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="8" t="s">
         <v>270</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="8" t="s">
         <v>208</v>
       </c>
     </row>
@@ -3603,10 +3617,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="6"/>
     </row>
     <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -3620,10 +3634,10 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="6"/>
     </row>
     <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -3757,7 +3771,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>218</v>
       </c>
@@ -3815,10 +3829,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" s="6"/>
     </row>
     <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -3862,7 +3876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
@@ -3918,10 +3932,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="6"/>
     </row>
     <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -4075,8 +4089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4131,10 +4145,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>415</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="6"/>
     </row>
     <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -4180,14 +4194,14 @@
         <v>230</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="8" t="s">
         <v>232</v>
       </c>
     </row>
@@ -4204,7 +4218,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4316,14 +4330,14 @@
         <v>331</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="8" t="s">
         <v>312</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="8" t="s">
         <v>188</v>
       </c>
     </row>
@@ -4532,10 +4546,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>361</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" s="6"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -4947,10 +4961,10 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="6" t="s">
         <v>357</v>
       </c>
-      <c r="B24" s="5"/>
+      <c r="B24" s="6"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -4964,10 +4978,10 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="5"/>
+      <c r="B26" s="6"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -4980,33 +4994,33 @@
         <v>355</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
+    <row r="28" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="5" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
+    <row r="29" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="5" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="B30" s="5"/>
+      <c r="B30" s="6"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
@@ -5032,19 +5046,19 @@
         <v>361</v>
       </c>
     </row>
-    <row r="34" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="7" t="s">
+    <row r="34" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="5" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B35" s="5"/>
+      <c r="B35" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Mid replacing folate with mpt
</commit_message>
<xml_diff>
--- a/Matt_Work/AA paths/All_Paths_formatted.xlsx
+++ b/Matt_Work/AA paths/All_Paths_formatted.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="10500" windowHeight="5832" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="10500" windowHeight="5835" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Summary and notes" sheetId="1" r:id="rId1"/>
@@ -1291,7 +1291,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1303,6 +1303,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1346,7 +1353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1365,6 +1372,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1704,15 +1712,15 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1867,18 +1875,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="115.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="123.85546875" customWidth="1"/>
+    <col min="3" max="3" width="54.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>391</v>
       </c>
@@ -1889,7 +1897,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1900,7 +1908,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1911,7 +1919,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1922,7 +1930,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -1933,7 +1941,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -1944,7 +1952,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -1955,7 +1963,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -1966,7 +1974,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -1977,7 +1985,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -1988,13 +1996,13 @@
         <v>364</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>73</v>
       </c>
       <c r="B11" s="8"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>74</v>
       </c>
@@ -2005,7 +2013,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>76</v>
       </c>
@@ -2016,7 +2024,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>78</v>
       </c>
@@ -2027,7 +2035,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>80</v>
       </c>
@@ -2038,7 +2046,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>82</v>
       </c>
@@ -2049,7 +2057,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>83</v>
       </c>
@@ -2060,7 +2068,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>84</v>
       </c>
@@ -2071,7 +2079,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>86</v>
       </c>
@@ -2082,18 +2090,18 @@
         <v>370</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="20" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="10" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>90</v>
       </c>
@@ -2104,7 +2112,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>92</v>
       </c>
@@ -2115,7 +2123,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>94</v>
       </c>
@@ -2126,7 +2134,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>96</v>
       </c>
@@ -2137,7 +2145,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>98</v>
       </c>
@@ -2153,6 +2161,7 @@
     <mergeCell ref="A11:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2164,14 +2173,14 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>391</v>
       </c>
@@ -2182,7 +2191,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2193,7 +2202,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2204,7 +2213,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2215,13 +2224,13 @@
         <v>331</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>101</v>
       </c>
       <c r="B5" s="8"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>102</v>
       </c>
@@ -2232,7 +2241,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>104</v>
       </c>
@@ -2243,7 +2252,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>106</v>
       </c>
@@ -2254,7 +2263,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>108</v>
       </c>
@@ -2265,13 +2274,13 @@
         <v>378</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>110</v>
       </c>
       <c r="B10" s="8"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>111</v>
       </c>
@@ -2282,7 +2291,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>113</v>
       </c>
@@ -2293,7 +2302,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>115</v>
       </c>
@@ -2304,7 +2313,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>117</v>
       </c>
@@ -2332,14 +2341,14 @@
       <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>391</v>
       </c>
@@ -2350,7 +2359,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2361,7 +2370,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2372,7 +2381,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2383,13 +2392,13 @@
         <v>331</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>120</v>
       </c>
       <c r="B5" s="8"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>121</v>
       </c>
@@ -2400,7 +2409,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>123</v>
       </c>
@@ -2411,7 +2420,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>125</v>
       </c>
@@ -2422,7 +2431,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>127</v>
       </c>
@@ -2433,7 +2442,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>129</v>
       </c>
@@ -2444,7 +2453,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>131</v>
       </c>
@@ -2455,7 +2464,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>133</v>
       </c>
@@ -2466,7 +2475,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>135</v>
       </c>
@@ -2477,7 +2486,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>137</v>
       </c>
@@ -2485,7 +2494,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>139</v>
       </c>
@@ -2512,14 +2521,14 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="80.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>391</v>
       </c>
@@ -2530,7 +2539,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2541,7 +2550,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2552,7 +2561,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2563,13 +2572,13 @@
         <v>331</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>142</v>
       </c>
       <c r="B5" s="8"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -2580,7 +2589,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -2591,13 +2600,13 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>143</v>
       </c>
       <c r="B8" s="8"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>144</v>
       </c>
@@ -2608,7 +2617,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>146</v>
       </c>
@@ -2619,7 +2628,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>148</v>
       </c>
@@ -2630,7 +2639,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>150</v>
       </c>
@@ -2641,7 +2650,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>152</v>
       </c>
@@ -2669,14 +2678,14 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="88.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="88.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>391</v>
       </c>
@@ -2687,7 +2696,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2698,7 +2707,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2709,7 +2718,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2720,7 +2729,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -2731,7 +2740,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -2742,7 +2751,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -2753,7 +2762,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -2764,13 +2773,13 @@
         <v>354</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>53</v>
       </c>
       <c r="B9" s="8"/>
     </row>
-    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -2781,7 +2790,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -2789,7 +2798,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -2800,7 +2809,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -2811,7 +2820,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -2822,7 +2831,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>155</v>
       </c>
@@ -2833,7 +2842,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>156</v>
       </c>
@@ -2841,13 +2850,13 @@
         <v>289</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>413</v>
       </c>
       <c r="B17" s="8"/>
     </row>
-    <row r="18" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>157</v>
       </c>
@@ -2855,7 +2864,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>158</v>
       </c>
@@ -2866,7 +2875,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>57</v>
       </c>
@@ -2895,14 +2904,14 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="112.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="112.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>391</v>
       </c>
@@ -2913,7 +2922,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2924,7 +2933,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2935,7 +2944,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2946,13 +2955,13 @@
         <v>331</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>414</v>
       </c>
       <c r="B5" s="8"/>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -2963,7 +2972,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>162</v>
       </c>
@@ -2974,7 +2983,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>164</v>
       </c>
@@ -2985,7 +2994,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>166</v>
       </c>
@@ -2996,7 +3005,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>168</v>
       </c>
@@ -3007,7 +3016,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>170</v>
       </c>
@@ -3018,7 +3027,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>69</v>
       </c>
@@ -3029,7 +3038,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>173</v>
       </c>
@@ -3040,7 +3049,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>175</v>
       </c>
@@ -3051,7 +3060,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>177</v>
       </c>
@@ -3059,7 +3068,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>178</v>
       </c>
@@ -3070,7 +3079,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>179</v>
       </c>
@@ -3097,14 +3106,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="100.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>391</v>
       </c>
@@ -3115,7 +3124,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3126,7 +3135,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3137,7 +3146,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3148,13 +3157,13 @@
         <v>331</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>182</v>
       </c>
       <c r="B5" s="8"/>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -3165,7 +3174,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -3176,7 +3185,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>185</v>
       </c>
@@ -3187,7 +3196,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>187</v>
       </c>
@@ -3198,7 +3207,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>189</v>
       </c>
@@ -3222,14 +3231,14 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="123.6640625" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="123.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>391</v>
       </c>
@@ -3240,7 +3249,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3251,7 +3260,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3262,7 +3271,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3302,7 +3311,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>70</v>
       </c>
@@ -3319,7 +3328,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>71</v>
       </c>
@@ -3336,7 +3345,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>68</v>
       </c>
@@ -3353,7 +3362,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>72</v>
       </c>
@@ -3365,7 +3374,7 @@
       </c>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -3376,7 +3385,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -3387,7 +3396,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>194</v>
       </c>
@@ -3398,7 +3407,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>196</v>
       </c>
@@ -3409,7 +3418,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" s="7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>198</v>
       </c>
@@ -3437,14 +3446,14 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="92.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>391</v>
       </c>
@@ -3455,7 +3464,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3466,7 +3475,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3477,7 +3486,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3488,13 +3497,13 @@
         <v>331</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>201</v>
       </c>
       <c r="B5" s="8"/>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -3505,7 +3514,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -3516,7 +3525,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -3527,7 +3536,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>205</v>
       </c>
@@ -3538,7 +3547,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>207</v>
       </c>
@@ -3565,14 +3574,14 @@
       <selection activeCell="A2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="113" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>391</v>
       </c>
@@ -3583,7 +3592,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3594,7 +3603,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3605,7 +3614,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3616,13 +3625,13 @@
         <v>331</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>210</v>
       </c>
       <c r="B5" s="8"/>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -3633,13 +3642,13 @@
         <v>211</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>160</v>
       </c>
       <c r="B7" s="8"/>
     </row>
-    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>74</v>
       </c>
@@ -3650,7 +3659,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>162</v>
       </c>
@@ -3661,7 +3670,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>164</v>
       </c>
@@ -3672,7 +3681,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>166</v>
       </c>
@@ -3683,7 +3692,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>168</v>
       </c>
@@ -3694,7 +3703,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>170</v>
       </c>
@@ -3705,7 +3714,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -3716,7 +3725,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>173</v>
       </c>
@@ -3727,7 +3736,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>175</v>
       </c>
@@ -3738,7 +3747,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>212</v>
       </c>
@@ -3749,7 +3758,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>214</v>
       </c>
@@ -3760,7 +3769,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>216</v>
       </c>
@@ -3771,7 +3780,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>218</v>
       </c>
@@ -3782,7 +3791,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>220</v>
       </c>
@@ -3810,14 +3819,14 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="88.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="88.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>391</v>
       </c>
@@ -3828,13 +3837,13 @@
         <v>328</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="8"/>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>319</v>
       </c>
@@ -3845,7 +3854,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>321</v>
       </c>
@@ -3853,7 +3862,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>323</v>
       </c>
@@ -3880,14 +3889,14 @@
       <selection activeCell="A2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="112.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="112.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>391</v>
       </c>
@@ -3898,7 +3907,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3909,7 +3918,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3920,7 +3929,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3931,13 +3940,13 @@
         <v>331</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>223</v>
       </c>
       <c r="B5" s="8"/>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -3948,7 +3957,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -3959,7 +3968,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>162</v>
       </c>
@@ -3970,7 +3979,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>164</v>
       </c>
@@ -3981,7 +3990,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>166</v>
       </c>
@@ -3992,7 +4001,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>168</v>
       </c>
@@ -4003,7 +4012,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>170</v>
       </c>
@@ -4014,7 +4023,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -4025,7 +4034,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>173</v>
       </c>
@@ -4036,7 +4045,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>175</v>
       </c>
@@ -4047,7 +4056,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>177</v>
       </c>
@@ -4055,7 +4064,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>224</v>
       </c>
@@ -4066,7 +4075,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>226</v>
       </c>
@@ -4093,14 +4102,14 @@
       <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="77" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>391</v>
       </c>
@@ -4111,7 +4120,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4122,7 +4131,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -4133,7 +4142,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -4144,13 +4153,13 @@
         <v>331</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>415</v>
       </c>
       <c r="B5" s="8"/>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>121</v>
       </c>
@@ -4161,7 +4170,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>123</v>
       </c>
@@ -4172,7 +4181,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>125</v>
       </c>
@@ -4183,7 +4192,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>127</v>
       </c>
@@ -4194,7 +4203,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>231</v>
       </c>
@@ -4221,14 +4230,14 @@
       <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="93.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="93.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>391</v>
       </c>
@@ -4239,7 +4248,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4250,7 +4259,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -4264,7 +4273,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -4275,7 +4284,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>302</v>
       </c>
@@ -4286,7 +4295,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>304</v>
       </c>
@@ -4297,7 +4306,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>305</v>
       </c>
@@ -4308,7 +4317,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>307</v>
       </c>
@@ -4319,7 +4328,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>309</v>
       </c>
@@ -4330,7 +4339,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>311</v>
       </c>
@@ -4341,7 +4350,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>313</v>
       </c>
@@ -4352,7 +4361,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>315</v>
       </c>
@@ -4363,7 +4372,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>317</v>
       </c>
@@ -4387,14 +4396,14 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>391</v>
       </c>
@@ -4405,7 +4414,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4416,7 +4425,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -4427,7 +4436,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -4438,7 +4447,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -4463,14 +4472,14 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>391</v>
       </c>
@@ -4481,7 +4490,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4492,7 +4501,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -4503,7 +4512,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -4527,11 +4536,11 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -4575,14 +4584,14 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>391</v>
       </c>
@@ -4593,7 +4602,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4604,7 +4613,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -4615,7 +4624,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -4639,14 +4648,14 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>391</v>
       </c>
@@ -4657,7 +4666,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4668,7 +4677,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -4679,7 +4688,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -4699,18 +4708,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="102.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="102.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>391</v>
       </c>
@@ -4721,7 +4730,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4732,7 +4741,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -4743,7 +4752,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -4754,7 +4763,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -4765,7 +4774,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -4776,7 +4785,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -4787,7 +4796,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -4798,7 +4807,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -4809,7 +4818,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>343</v>
       </c>
@@ -4820,7 +4829,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -4831,7 +4840,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -4842,7 +4851,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -4853,7 +4862,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -4864,7 +4873,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -4875,7 +4884,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -4886,7 +4895,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -4897,7 +4906,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>300</v>
       </c>
@@ -4908,7 +4917,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -4919,7 +4928,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -4930,7 +4939,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -4941,7 +4950,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -4949,7 +4958,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -4960,13 +4969,13 @@
         <v>353</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>357</v>
       </c>
       <c r="B24" s="8"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -4977,13 +4986,13 @@
         <v>354</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>53</v>
       </c>
       <c r="B26" s="8"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -4994,7 +5003,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>158</v>
       </c>
@@ -5005,7 +5014,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>57</v>
       </c>
@@ -5016,13 +5025,13 @@
         <v>358</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>359</v>
       </c>
       <c r="B30" s="8"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>59</v>
       </c>
@@ -5030,7 +5039,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -5041,12 +5050,12 @@
         <v>360</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="34" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>63</v>
       </c>
@@ -5054,7 +5063,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
         <v>65</v>
       </c>

</xml_diff>